<commit_message>
ADD EVENT ON EXCEL
</commit_message>
<xml_diff>
--- a/Luban/Config/Datas/Root/EventConfig.xlsx
+++ b/Luban/Config/Datas/Root/EventConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Game\RootsPinkShark\Luban\Config\Datas\Root\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73E736B-FC67-4FE9-92D2-C098B712A6AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3EBE59-AEBA-4C22-9575-1275DB692E26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6915" yWindow="2850" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Event" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="87">
   <si>
     <t>##</t>
   </si>
@@ -251,10 +251,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Age</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>结婚</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -288,6 +284,92 @@
   </si>
   <si>
     <t>GROWTH,1,0;GROWTH,1,1;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>佳偶天成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>意外身故</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>痛失爱子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>明镜高悬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsOnBase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否在初始事件库</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>偶得机缘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>初窥门径</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登堂入室</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>富甲一方</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小有进财</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>你找到了配偶</t>
+  </si>
+  <si>
+    <t>DIE,0,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADD_RESOURCE,0,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DIE_SON,0,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AGE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HAS_CHILDREN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADD_MONEY,100,0</t>
+  </si>
+  <si>
+    <t>ADD_MONEY,100,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADD_MONEY,10,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADD_CURR_EVENT,11,1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADD_CURR_EVENT,14,1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -624,15 +706,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -669,8 +751,11 @@
       <c r="L1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -699,16 +784,19 @@
         <v>12</v>
       </c>
       <c r="J2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+      <c r="M2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -745,8 +833,11 @@
       <c r="L3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>53</v>
       </c>
@@ -772,18 +863,21 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+      <c r="M4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
         <v>57</v>
-      </c>
-      <c r="C5" t="s">
-        <v>58</v>
       </c>
       <c r="D5" t="s">
         <v>55</v>
@@ -804,10 +898,301 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L5" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="M5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" t="s">
+        <v>63</v>
+      </c>
+      <c r="M6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" t="s">
+        <v>77</v>
+      </c>
+      <c r="M7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8" t="s">
+        <v>79</v>
+      </c>
+      <c r="M8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+      <c r="L9" t="s">
+        <v>78</v>
+      </c>
+      <c r="M9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10">
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L10" t="s">
+        <v>85</v>
+      </c>
+      <c r="M10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+      <c r="L11" t="s">
+        <v>86</v>
+      </c>
+      <c r="M11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12">
+        <v>9</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12" t="s">
+        <v>82</v>
+      </c>
+      <c r="M12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13">
+        <v>10</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="L13" t="s">
+        <v>84</v>
+      </c>
+      <c r="M13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14">
+        <v>11</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14" t="s">
+        <v>83</v>
+      </c>
+      <c r="M14" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -818,10 +1203,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CF7FC9E-1911-4063-8600-A529D48BB6E9}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -870,13 +1255,24 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="C4">
         <v>10</v>
       </c>
       <c r="D4">
         <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -984,7 +1380,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add New Excel Structure
</commit_message>
<xml_diff>
--- a/Luban/Config/Datas/Root/EventConfig.xlsx
+++ b/Luban/Config/Datas/Root/EventConfig.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Game\RootsPinkShark\Luban\Config\Datas\Root\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B1179A-3F51-4185-A765-5982D35311D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89133969-F99F-43C7-9B11-E3C07A448868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="1230" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="5160" windowWidth="21600" windowHeight="10155" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Event" sheetId="1" r:id="rId1"/>
     <sheet name="EventCondition" sheetId="4" r:id="rId2"/>
     <sheet name="EventOption" sheetId="2" r:id="rId3"/>
-    <sheet name="EventEffect" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="105">
   <si>
     <t>##</t>
   </si>
@@ -116,25 +115,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>list, EventEffect</t>
-  </si>
-  <si>
     <t>是否是可交互事件</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>EventOptionName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>EventOptionDesc</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>选项名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>选项描述</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -163,10 +151,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>OptionLoseEffect</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>OptionWinEffect</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -175,10 +159,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>失败效果</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>事件结果（非交互事件才需要）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -187,18 +167,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>EventEffectType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EffectType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>效果类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Para1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -219,10 +187,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>list,EventCondition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>出现条件</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -231,10 +195,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>list,ResourceType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>EventConditionName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -259,22 +219,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>(list#sep=;),EventOption</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Adult,0,0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>(list#sep=;),EventCondition#sep=,</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>young,0,0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>(list#sep=;), EventEffect#sep=,</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -346,10 +294,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>AGE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>HAS_CHILDREN</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -370,6 +314,134 @@
   </si>
   <si>
     <t>ADD_CURR_EVENT,14,1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>路障</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>路上遇到了一块巨石挡路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>仙人指路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>仙人告知了你天地仅存的一处洞天福地</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>触发了仙缘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>THIS_HAVEDONE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALL_HAVEDONE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALL_HAVEDONE,11,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>选项id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>利用灵力催发冲击，破坏石头</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EventOptionid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>浑身包裹鬼气穿过石头</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATTRIMINNEED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,0,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OptionDES</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>成功效果说明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HAVETAG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AGEBETWEEN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HAVERES</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATTRIMINNEED,1,5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATTRIMINNEED,5,2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADD_RESOURCE,0,1;ADD_RESOURCE,1,1;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用灵力震碎了石头，意外获得了几块金币</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GROWTH,3,1;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>隐约瞧见了石头的内壁上写了文字，一股记忆传入脑海</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(list#sep=;), EventCondition#sep=,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(list#sep=;),int#ref=TbEventOption</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EffectCondition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AGEBETWEEN,0,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AGEBETWEEN,10,20;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(list#sep=,),ResourceType</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -401,12 +473,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -421,10 +499,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -706,13 +795,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="36.5" customWidth="1"/>
+    <col min="4" max="4" width="16.75" customWidth="1"/>
+    <col min="5" max="5" width="8.375" customWidth="1"/>
+    <col min="6" max="6" width="13.875" customWidth="1"/>
+    <col min="7" max="7" width="14.375" customWidth="1"/>
+    <col min="8" max="8" width="13.75" customWidth="1"/>
+    <col min="9" max="9" width="17.875" customWidth="1"/>
+    <col min="10" max="10" width="19.25" customWidth="1"/>
+    <col min="11" max="11" width="24.625" customWidth="1"/>
+    <col min="12" max="12" width="32.125" customWidth="1"/>
+    <col min="13" max="13" width="18.875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -743,7 +845,7 @@
         <v>19</v>
       </c>
       <c r="J1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="K1" t="s">
         <v>20</v>
@@ -752,7 +854,7 @@
         <v>21</v>
       </c>
       <c r="M1" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -784,13 +886,13 @@
         <v>12</v>
       </c>
       <c r="J2" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="K2" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="L2" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="M2" t="s">
         <v>12</v>
@@ -822,30 +924,30 @@
         <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J3" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="K3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="L3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="M3" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -863,10 +965,10 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>61</v>
+        <v>102</v>
       </c>
       <c r="L4" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="M4" t="b">
         <v>1</v>
@@ -874,13 +976,13 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -898,10 +1000,10 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>59</v>
+        <v>102</v>
       </c>
       <c r="L5" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="M5" t="b">
         <v>1</v>
@@ -909,13 +1011,13 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -932,8 +1034,11 @@
       <c r="I6" t="b">
         <v>0</v>
       </c>
+      <c r="J6" t="s">
+        <v>103</v>
+      </c>
       <c r="L6" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="M6" t="b">
         <v>1</v>
@@ -941,13 +1046,13 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E7">
         <v>4</v>
@@ -965,7 +1070,7 @@
         <v>0</v>
       </c>
       <c r="L7" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="M7" t="b">
         <v>1</v>
@@ -973,13 +1078,13 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E8">
         <v>5</v>
@@ -997,7 +1102,7 @@
         <v>0</v>
       </c>
       <c r="L8" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="M8" t="b">
         <v>1</v>
@@ -1005,13 +1110,13 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E9">
         <v>6</v>
@@ -1029,7 +1134,7 @@
         <v>0</v>
       </c>
       <c r="L9" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="M9" t="b">
         <v>1</v>
@@ -1037,13 +1142,13 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E10">
         <v>7</v>
@@ -1061,21 +1166,21 @@
         <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="M10" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E11">
         <v>8</v>
@@ -1093,7 +1198,7 @@
         <v>0</v>
       </c>
       <c r="L11" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="M11" t="b">
         <v>0</v>
@@ -1101,13 +1206,13 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E12">
         <v>9</v>
@@ -1125,7 +1230,7 @@
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="M12" t="b">
         <v>1</v>
@@ -1133,13 +1238,13 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E13">
         <v>10</v>
@@ -1157,7 +1262,7 @@
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="M13" t="b">
         <v>1</v>
@@ -1165,13 +1270,13 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E14">
         <v>11</v>
@@ -1189,9 +1294,77 @@
         <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="M14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15">
+        <v>12</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" t="b">
+        <v>1</v>
+      </c>
+      <c r="K15" t="s">
+        <v>84</v>
+      </c>
+      <c r="L15" s="2"/>
+      <c r="M15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16">
+        <v>13</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>80</v>
+      </c>
+      <c r="L16" t="s">
+        <v>65</v>
+      </c>
+      <c r="M16" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1203,34 +1376,43 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CF7FC9E-1911-4063-8600-A529D48BB6E9}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="23.875" customWidth="1"/>
+    <col min="3" max="3" width="13.75" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="19.25" customWidth="1"/>
+    <col min="6" max="6" width="9.75" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>101</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1238,40 +1420,97 @@
       <c r="D2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
         <v>0</v>
       </c>
     </row>
@@ -1283,148 +1522,140 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D8AFCC-95AF-4A6B-815E-C005352AB991}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="17.625" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="17.75" customWidth="1"/>
+    <col min="5" max="5" width="26.125" customWidth="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1"/>
+    <col min="7" max="7" width="26.375" customWidth="1"/>
+    <col min="8" max="8" width="18.5" customWidth="1"/>
+    <col min="9" max="9" width="21.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>24</v>
+      <c r="B1" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s">
-        <v>28</v>
-      </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" t="s">
-        <v>34</v>
+        <v>31</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
+      <c r="B2" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" t="s">
-        <v>48</v>
+      <c r="D2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="F2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
+        <v>104</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5E07438-828D-4559-A9CD-524CF68240CF}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" t="s">
-        <v>46</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="6">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H5" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Most of Functionality
</commit_message>
<xml_diff>
--- a/Luban/Config/Datas/Root/EventConfig.xlsx
+++ b/Luban/Config/Datas/Root/EventConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Game\RootsPinkShark\Luban\Config\Datas\Root\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89133969-F99F-43C7-9B11-E3C07A448868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358DA0D0-1D9D-4DE4-9916-465E999B4BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="5160" windowWidth="21600" windowHeight="10155" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3210" yWindow="3795" windowWidth="21600" windowHeight="10155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Event" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="114">
   <si>
     <t>##</t>
   </si>
@@ -279,17 +279,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>你找到了配偶</t>
-  </si>
-  <si>
     <t>DIE,0,0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ADD_RESOURCE,0,0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DIE_SON,0,0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -433,15 +426,59 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>AGEBETWEEN,0,0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>AGEBETWEEN,10,20;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>(list#sep=,),ResourceType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>你获得了一个宝贝~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADD_RESOURCE,1,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>你找到了很棒的配偶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>你死了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>你儿子死了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>你白了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>你得到了机缘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>你读书很厉害</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>你赚了点小钱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>你赚了很多</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MARRY,0,0;TAGACTIVE,1,0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -795,10 +832,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -889,7 +926,7 @@
         <v>48</v>
       </c>
       <c r="K2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="L2" t="s">
         <v>49</v>
@@ -964,9 +1001,6 @@
       <c r="I4" t="b">
         <v>0</v>
       </c>
-      <c r="J4" t="s">
-        <v>102</v>
-      </c>
       <c r="L4" t="s">
         <v>51</v>
       </c>
@@ -999,11 +1033,8 @@
       <c r="I5" t="b">
         <v>0</v>
       </c>
-      <c r="J5" t="s">
-        <v>102</v>
-      </c>
       <c r="L5" t="s">
-        <v>50</v>
+        <v>113</v>
       </c>
       <c r="M5" t="b">
         <v>1</v>
@@ -1014,7 +1045,7 @@
         <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="D6" t="s">
         <v>45</v>
@@ -1035,7 +1066,7 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="L6" t="s">
         <v>50</v>
@@ -1049,7 +1080,7 @@
         <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="D7" t="s">
         <v>45</v>
@@ -1070,7 +1101,7 @@
         <v>0</v>
       </c>
       <c r="L7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M7" t="b">
         <v>1</v>
@@ -1081,7 +1112,7 @@
         <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="D8" t="s">
         <v>45</v>
@@ -1093,7 +1124,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
@@ -1102,7 +1133,7 @@
         <v>0</v>
       </c>
       <c r="L8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M8" t="b">
         <v>1</v>
@@ -1113,7 +1144,7 @@
         <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>108</v>
       </c>
       <c r="D9" t="s">
         <v>45</v>
@@ -1134,7 +1165,7 @@
         <v>0</v>
       </c>
       <c r="L9" t="s">
-        <v>65</v>
+        <v>104</v>
       </c>
       <c r="M9" t="b">
         <v>1</v>
@@ -1145,7 +1176,7 @@
         <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>109</v>
       </c>
       <c r="D10" t="s">
         <v>45</v>
@@ -1166,7 +1197,7 @@
         <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M10" t="b">
         <v>1</v>
@@ -1177,7 +1208,7 @@
         <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D11" t="s">
         <v>45</v>
@@ -1198,7 +1229,7 @@
         <v>0</v>
       </c>
       <c r="L11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M11" t="b">
         <v>0</v>
@@ -1209,7 +1240,7 @@
         <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="D12" t="s">
         <v>45</v>
@@ -1230,7 +1261,7 @@
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M12" t="b">
         <v>1</v>
@@ -1241,7 +1272,7 @@
         <v>62</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>111</v>
       </c>
       <c r="D13" t="s">
         <v>45</v>
@@ -1262,7 +1293,7 @@
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M13" t="b">
         <v>1</v>
@@ -1273,7 +1304,7 @@
         <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>112</v>
       </c>
       <c r="D14" t="s">
         <v>45</v>
@@ -1294,7 +1325,7 @@
         <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M14" t="b">
         <v>0</v>
@@ -1302,10 +1333,10 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D15" t="s">
         <v>45</v>
@@ -1326,7 +1357,7 @@
         <v>1</v>
       </c>
       <c r="K15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15" t="b">
@@ -1335,10 +1366,10 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D16" t="s">
         <v>45</v>
@@ -1359,13 +1390,45 @@
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L16" t="s">
-        <v>65</v>
+        <v>104</v>
       </c>
       <c r="M16" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17">
+        <v>14</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" t="b">
+        <v>0</v>
+      </c>
+      <c r="L17" t="s">
+        <v>104</v>
+      </c>
+      <c r="M17" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1412,7 +1475,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1439,7 +1502,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1450,7 +1513,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1461,7 +1524,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1472,7 +1535,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1483,7 +1546,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1494,7 +1557,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1505,7 +1568,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1524,7 +1587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D8AFCC-95AF-4A6B-815E-C005352AB991}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -1545,7 +1608,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C1" t="s">
         <v>23</v>
@@ -1563,7 +1626,7 @@
         <v>31</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1577,13 +1640,13 @@
         <v>2</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>49</v>
@@ -1597,7 +1660,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
@@ -1615,7 +1678,7 @@
         <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1623,19 +1686,19 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" t="s">
         <v>93</v>
       </c>
-      <c r="F4" t="s">
-        <v>87</v>
-      </c>
-      <c r="G4" t="s">
-        <v>95</v>
-      </c>
       <c r="H4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1643,19 +1706,19 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F5" t="s">
         <v>85</v>
       </c>
-      <c r="E5" t="s">
-        <v>94</v>
-      </c>
-      <c r="F5" t="s">
-        <v>87</v>
-      </c>
       <c r="G5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Bugs on Events
</commit_message>
<xml_diff>
--- a/Luban/Config/Datas/Root/EventConfig.xlsx
+++ b/Luban/Config/Datas/Root/EventConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Game\RootsPinkShark\Luban\Config\Datas\Root\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E8266A-4702-4D54-B0C6-820C2D4EC72C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F833FD-83E4-40E5-9F39-883282B7E759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10305" yWindow="1980" windowWidth="21600" windowHeight="10155" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Event" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="416">
   <si>
     <t>##</t>
   </si>
@@ -958,10 +958,6 @@
   </si>
   <si>
     <t>25,26</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>68,69,70</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1996,8 +1992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O145"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="D103" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L108" sqref="L108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2099,7 +2095,7 @@
         <v>41</v>
       </c>
       <c r="L2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="M2" t="s">
         <v>42</v>
@@ -2184,7 +2180,7 @@
         <v>99</v>
       </c>
       <c r="M4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="N4" t="b">
         <v>1</v>
@@ -2245,7 +2241,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>187</v>
@@ -2479,7 +2475,7 @@
         <v>179</v>
       </c>
       <c r="L12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="N12" t="b">
         <v>1</v>
@@ -2514,7 +2510,7 @@
         <v>178</v>
       </c>
       <c r="L13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N13" t="b">
         <v>1</v>
@@ -2549,7 +2545,7 @@
         <v>177</v>
       </c>
       <c r="L14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N14" t="b">
         <v>1</v>
@@ -2581,7 +2577,7 @@
         <v>99</v>
       </c>
       <c r="K15" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="M15" t="s">
         <v>46</v>
@@ -2595,7 +2591,7 @@
         <v>62</v>
       </c>
       <c r="C16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E16">
         <v>13</v>
@@ -2616,7 +2612,7 @@
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="M16" t="s">
         <v>212</v>
@@ -2633,7 +2629,7 @@
         <v>63</v>
       </c>
       <c r="C17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E17">
         <v>14</v>
@@ -2654,7 +2650,7 @@
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="M17" t="s">
         <v>213</v>
@@ -2671,7 +2667,7 @@
         <v>181</v>
       </c>
       <c r="C18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E18">
         <v>15</v>
@@ -2692,7 +2688,7 @@
         <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="M18" t="s">
         <v>214</v>
@@ -2709,7 +2705,7 @@
         <v>64</v>
       </c>
       <c r="C19" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E19">
         <v>16</v>
@@ -2730,7 +2726,7 @@
         <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="M19" t="s">
         <v>215</v>
@@ -2747,7 +2743,7 @@
         <v>65</v>
       </c>
       <c r="C20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E20">
         <v>17</v>
@@ -2785,7 +2781,7 @@
         <v>66</v>
       </c>
       <c r="C21" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E21">
         <v>18</v>
@@ -2823,7 +2819,7 @@
         <v>67</v>
       </c>
       <c r="C22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E22">
         <v>19</v>
@@ -2861,7 +2857,7 @@
         <v>68</v>
       </c>
       <c r="C23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E23">
         <v>20</v>
@@ -2899,7 +2895,7 @@
         <v>69</v>
       </c>
       <c r="C24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E24">
         <v>21</v>
@@ -2937,7 +2933,7 @@
         <v>70</v>
       </c>
       <c r="C25" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E25">
         <v>22</v>
@@ -2975,7 +2971,7 @@
         <v>71</v>
       </c>
       <c r="C26" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E26">
         <v>23</v>
@@ -3013,7 +3009,7 @@
         <v>72</v>
       </c>
       <c r="C27" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E27">
         <v>24</v>
@@ -3048,10 +3044,10 @@
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C28" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E28">
         <v>25</v>
@@ -3086,10 +3082,10 @@
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C29" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E29">
         <v>26</v>
@@ -3124,10 +3120,10 @@
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E30">
         <v>27</v>
@@ -3165,7 +3161,7 @@
         <v>73</v>
       </c>
       <c r="C31" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E31">
         <v>28</v>
@@ -3203,7 +3199,7 @@
         <v>74</v>
       </c>
       <c r="C32" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E32">
         <v>29</v>
@@ -3241,7 +3237,7 @@
         <v>75</v>
       </c>
       <c r="C33" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E33">
         <v>30</v>
@@ -3279,7 +3275,7 @@
         <v>76</v>
       </c>
       <c r="C34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E34">
         <v>31</v>
@@ -3431,7 +3427,7 @@
         <v>82</v>
       </c>
       <c r="C38" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E38">
         <v>35</v>
@@ -3469,7 +3465,7 @@
         <v>83</v>
       </c>
       <c r="C39" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E39">
         <v>36</v>
@@ -3507,7 +3503,7 @@
         <v>84</v>
       </c>
       <c r="C40" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E40">
         <v>37</v>
@@ -3545,7 +3541,7 @@
         <v>85</v>
       </c>
       <c r="C41" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E41">
         <v>38</v>
@@ -3583,7 +3579,7 @@
         <v>86</v>
       </c>
       <c r="C42" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E42">
         <v>39</v>
@@ -3618,10 +3614,10 @@
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C43" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E43">
         <v>40</v>
@@ -3656,10 +3652,10 @@
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C44" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E44">
         <v>41</v>
@@ -3694,10 +3690,10 @@
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C45" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E45">
         <v>42</v>
@@ -3732,10 +3728,10 @@
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C46" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E46">
         <v>43</v>
@@ -3770,10 +3766,10 @@
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C47" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E47">
         <v>44</v>
@@ -3808,10 +3804,10 @@
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C48" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E48">
         <v>45</v>
@@ -3846,10 +3842,10 @@
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C49" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E49">
         <v>46</v>
@@ -3873,16 +3869,19 @@
         <v>207</v>
       </c>
       <c r="M49" s="1"/>
+      <c r="N49" t="b">
+        <v>0</v>
+      </c>
       <c r="O49">
         <v>150</v>
       </c>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C50" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E50">
         <v>47</v>
@@ -3906,16 +3905,19 @@
         <v>207</v>
       </c>
       <c r="M50" s="1"/>
+      <c r="N50" t="b">
+        <v>0</v>
+      </c>
       <c r="O50">
         <v>150</v>
       </c>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C51" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E51">
         <v>48</v>
@@ -3939,16 +3941,19 @@
         <v>207</v>
       </c>
       <c r="M51" s="1"/>
+      <c r="N51" t="b">
+        <v>0</v>
+      </c>
       <c r="O51">
         <v>150</v>
       </c>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C52" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E52">
         <v>49</v>
@@ -3972,16 +3977,19 @@
         <v>208</v>
       </c>
       <c r="M52" s="1"/>
+      <c r="N52" t="b">
+        <v>0</v>
+      </c>
       <c r="O52">
         <v>150</v>
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C53" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E53">
         <v>50</v>
@@ -4005,16 +4013,19 @@
         <v>208</v>
       </c>
       <c r="M53" s="1"/>
+      <c r="N53" t="b">
+        <v>0</v>
+      </c>
       <c r="O53">
         <v>150</v>
       </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C54" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E54">
         <v>51</v>
@@ -4038,16 +4049,19 @@
         <v>208</v>
       </c>
       <c r="M54" s="1"/>
+      <c r="N54" t="b">
+        <v>0</v>
+      </c>
       <c r="O54">
         <v>150</v>
       </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C55" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E55">
         <v>52</v>
@@ -4071,16 +4085,19 @@
         <v>209</v>
       </c>
       <c r="M55" s="1"/>
+      <c r="N55" t="b">
+        <v>0</v>
+      </c>
       <c r="O55">
         <v>150</v>
       </c>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C56" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E56">
         <v>53</v>
@@ -4104,16 +4121,19 @@
         <v>209</v>
       </c>
       <c r="M56" s="1"/>
+      <c r="N56" t="b">
+        <v>0</v>
+      </c>
       <c r="O56">
         <v>150</v>
       </c>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C57" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E57">
         <v>54</v>
@@ -4137,6 +4157,9 @@
         <v>209</v>
       </c>
       <c r="M57" s="1"/>
+      <c r="N57" t="b">
+        <v>0</v>
+      </c>
       <c r="O57">
         <v>150</v>
       </c>
@@ -4170,7 +4193,7 @@
         <v>184</v>
       </c>
       <c r="L58" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="N58" t="b">
         <v>1</v>
@@ -4284,7 +4307,7 @@
         <v>184</v>
       </c>
       <c r="L61" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N61" t="b">
         <v>1</v>
@@ -4322,7 +4345,7 @@
         <v>184</v>
       </c>
       <c r="L62" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="N62" t="b">
         <v>1</v>
@@ -4360,7 +4383,7 @@
         <v>184</v>
       </c>
       <c r="L63" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="N63" t="b">
         <v>1</v>
@@ -4374,7 +4397,7 @@
         <v>93</v>
       </c>
       <c r="C64" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E64">
         <v>61</v>
@@ -4412,7 +4435,7 @@
         <v>94</v>
       </c>
       <c r="C65" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E65">
         <v>62</v>
@@ -4450,7 +4473,7 @@
         <v>95</v>
       </c>
       <c r="C66" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E66">
         <v>63</v>
@@ -4488,7 +4511,7 @@
         <v>96</v>
       </c>
       <c r="C67" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E67">
         <v>64</v>
@@ -4526,7 +4549,7 @@
         <v>97</v>
       </c>
       <c r="C68" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E68">
         <v>65</v>
@@ -4564,7 +4587,7 @@
         <v>98</v>
       </c>
       <c r="C69" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E69">
         <v>66</v>
@@ -4602,7 +4625,7 @@
         <v>99</v>
       </c>
       <c r="C70" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E70">
         <v>67</v>
@@ -4640,7 +4663,7 @@
         <v>100</v>
       </c>
       <c r="C71" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E71">
         <v>68</v>
@@ -4678,7 +4701,7 @@
         <v>101</v>
       </c>
       <c r="C72" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E72">
         <v>69</v>
@@ -4713,7 +4736,7 @@
         <v>102</v>
       </c>
       <c r="C73" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E73">
         <v>70</v>
@@ -4748,7 +4771,7 @@
         <v>103</v>
       </c>
       <c r="C74" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E74">
         <v>71</v>
@@ -4783,7 +4806,7 @@
         <v>104</v>
       </c>
       <c r="C75" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E75">
         <v>72</v>
@@ -4818,7 +4841,7 @@
         <v>105</v>
       </c>
       <c r="C76" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E76">
         <v>73</v>
@@ -4853,7 +4876,7 @@
         <v>106</v>
       </c>
       <c r="C77" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E77">
         <v>74</v>
@@ -4888,7 +4911,7 @@
         <v>107</v>
       </c>
       <c r="C78" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E78">
         <v>75</v>
@@ -4923,7 +4946,7 @@
         <v>108</v>
       </c>
       <c r="C79" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E79">
         <v>76</v>
@@ -4958,7 +4981,7 @@
         <v>109</v>
       </c>
       <c r="C80" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E80">
         <v>77</v>
@@ -4993,7 +5016,7 @@
         <v>110</v>
       </c>
       <c r="C81" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E81">
         <v>78</v>
@@ -5028,7 +5051,7 @@
         <v>111</v>
       </c>
       <c r="C82" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E82">
         <v>79</v>
@@ -5063,7 +5086,7 @@
         <v>112</v>
       </c>
       <c r="C83" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E83">
         <v>80</v>
@@ -5098,7 +5121,7 @@
         <v>113</v>
       </c>
       <c r="C84" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E84">
         <v>81</v>
@@ -5133,7 +5156,7 @@
         <v>114</v>
       </c>
       <c r="C85" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E85">
         <v>82</v>
@@ -5168,7 +5191,7 @@
         <v>115</v>
       </c>
       <c r="C86" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E86">
         <v>83</v>
@@ -5203,7 +5226,7 @@
         <v>116</v>
       </c>
       <c r="C87" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E87">
         <v>84</v>
@@ -5238,7 +5261,7 @@
         <v>117</v>
       </c>
       <c r="C88" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E88">
         <v>85</v>
@@ -5273,7 +5296,7 @@
         <v>118</v>
       </c>
       <c r="C89" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E89">
         <v>86</v>
@@ -5308,7 +5331,7 @@
         <v>119</v>
       </c>
       <c r="C90" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E90">
         <v>87</v>
@@ -5343,7 +5366,7 @@
         <v>120</v>
       </c>
       <c r="C91" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E91">
         <v>88</v>
@@ -5378,7 +5401,7 @@
         <v>121</v>
       </c>
       <c r="C92" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E92">
         <v>89</v>
@@ -5413,7 +5436,7 @@
         <v>122</v>
       </c>
       <c r="C93" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E93">
         <v>90</v>
@@ -5448,7 +5471,7 @@
         <v>123</v>
       </c>
       <c r="C94" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E94">
         <v>91</v>
@@ -5483,7 +5506,7 @@
         <v>124</v>
       </c>
       <c r="C95" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E95">
         <v>92</v>
@@ -5518,7 +5541,7 @@
         <v>125</v>
       </c>
       <c r="C96" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E96">
         <v>93</v>
@@ -5553,7 +5576,7 @@
         <v>126</v>
       </c>
       <c r="C97" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E97">
         <v>94</v>
@@ -5588,7 +5611,7 @@
         <v>127</v>
       </c>
       <c r="C98" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E98">
         <v>95</v>
@@ -5623,7 +5646,7 @@
         <v>128</v>
       </c>
       <c r="C99" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E99">
         <v>96</v>
@@ -5658,7 +5681,7 @@
         <v>121</v>
       </c>
       <c r="C100" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E100">
         <v>97</v>
@@ -5693,7 +5716,7 @@
         <v>122</v>
       </c>
       <c r="C101" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E101">
         <v>98</v>
@@ -5728,7 +5751,7 @@
         <v>123</v>
       </c>
       <c r="C102" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E102">
         <v>99</v>
@@ -5763,7 +5786,7 @@
         <v>124</v>
       </c>
       <c r="C103" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E103">
         <v>100</v>
@@ -5798,7 +5821,7 @@
         <v>125</v>
       </c>
       <c r="C104" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E104">
         <v>101</v>
@@ -5833,7 +5856,7 @@
         <v>126</v>
       </c>
       <c r="C105" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E105">
         <v>102</v>
@@ -5868,7 +5891,7 @@
         <v>127</v>
       </c>
       <c r="C106" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E106">
         <v>103</v>
@@ -5903,7 +5926,7 @@
         <v>128</v>
       </c>
       <c r="C107" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E107">
         <v>104</v>
@@ -5961,9 +5984,6 @@
       <c r="K108" t="s">
         <v>183</v>
       </c>
-      <c r="L108" t="s">
-        <v>240</v>
-      </c>
       <c r="N108" t="b">
         <v>1</v>
       </c>
@@ -6317,6 +6337,9 @@
       <c r="F118">
         <v>28</v>
       </c>
+      <c r="G118" t="b">
+        <v>1</v>
+      </c>
       <c r="H118" t="b">
         <v>1</v>
       </c>
@@ -6349,6 +6372,9 @@
       <c r="F119">
         <v>28</v>
       </c>
+      <c r="G119" t="b">
+        <v>1</v>
+      </c>
       <c r="H119" t="b">
         <v>1</v>
       </c>
@@ -6381,6 +6407,9 @@
       <c r="F120">
         <v>28</v>
       </c>
+      <c r="G120" t="b">
+        <v>1</v>
+      </c>
       <c r="H120" t="b">
         <v>1</v>
       </c>
@@ -6413,6 +6442,9 @@
       <c r="F121">
         <v>28</v>
       </c>
+      <c r="G121" t="b">
+        <v>1</v>
+      </c>
       <c r="H121" t="b">
         <v>1</v>
       </c>
@@ -6445,6 +6477,9 @@
       <c r="F122">
         <v>29</v>
       </c>
+      <c r="G122" t="b">
+        <v>1</v>
+      </c>
       <c r="H122" t="b">
         <v>1</v>
       </c>
@@ -6455,7 +6490,10 @@
         <v>0</v>
       </c>
       <c r="M122" t="s">
-        <v>373</v>
+        <v>372</v>
+      </c>
+      <c r="N122" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="2:15" x14ac:dyDescent="0.2">
@@ -6471,6 +6509,9 @@
       <c r="F123">
         <v>29</v>
       </c>
+      <c r="G123" t="b">
+        <v>1</v>
+      </c>
       <c r="H123" t="b">
         <v>1</v>
       </c>
@@ -6481,7 +6522,10 @@
         <v>0</v>
       </c>
       <c r="M123" t="s">
-        <v>374</v>
+        <v>373</v>
+      </c>
+      <c r="N123" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="2:15" x14ac:dyDescent="0.2">
@@ -6497,6 +6541,9 @@
       <c r="F124">
         <v>29</v>
       </c>
+      <c r="G124" t="b">
+        <v>1</v>
+      </c>
       <c r="H124" t="b">
         <v>1</v>
       </c>
@@ -6507,7 +6554,10 @@
         <v>0</v>
       </c>
       <c r="M124" t="s">
-        <v>375</v>
+        <v>374</v>
+      </c>
+      <c r="N124" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="2:15" x14ac:dyDescent="0.2">
@@ -6523,6 +6573,9 @@
       <c r="F125">
         <v>29</v>
       </c>
+      <c r="G125" t="b">
+        <v>1</v>
+      </c>
       <c r="H125" t="b">
         <v>1</v>
       </c>
@@ -6533,7 +6586,10 @@
         <v>0</v>
       </c>
       <c r="M125" t="s">
-        <v>376</v>
+        <v>375</v>
+      </c>
+      <c r="N125" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="2:15" x14ac:dyDescent="0.2">
@@ -6549,6 +6605,9 @@
       <c r="F126">
         <v>29</v>
       </c>
+      <c r="G126" t="b">
+        <v>1</v>
+      </c>
       <c r="H126" t="b">
         <v>1</v>
       </c>
@@ -6559,7 +6618,10 @@
         <v>0</v>
       </c>
       <c r="M126" t="s">
-        <v>377</v>
+        <v>376</v>
+      </c>
+      <c r="N126" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="2:15" x14ac:dyDescent="0.2">
@@ -6575,6 +6637,9 @@
       <c r="F127">
         <v>29</v>
       </c>
+      <c r="G127" t="b">
+        <v>1</v>
+      </c>
       <c r="H127" t="b">
         <v>1</v>
       </c>
@@ -6585,7 +6650,10 @@
         <v>0</v>
       </c>
       <c r="M127" t="s">
-        <v>378</v>
+        <v>377</v>
+      </c>
+      <c r="N127" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="2:15" x14ac:dyDescent="0.2">
@@ -6601,6 +6669,9 @@
       <c r="F128">
         <v>29</v>
       </c>
+      <c r="G128" t="b">
+        <v>1</v>
+      </c>
       <c r="H128" t="b">
         <v>1</v>
       </c>
@@ -6611,10 +6682,13 @@
         <v>0</v>
       </c>
       <c r="M128" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="129" spans="2:13" x14ac:dyDescent="0.2">
+        <v>378</v>
+      </c>
+      <c r="N128" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
         <v>150</v>
       </c>
@@ -6627,6 +6701,9 @@
       <c r="F129">
         <v>29</v>
       </c>
+      <c r="G129" t="b">
+        <v>1</v>
+      </c>
       <c r="H129" t="b">
         <v>1</v>
       </c>
@@ -6637,10 +6714,13 @@
         <v>0</v>
       </c>
       <c r="M129" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="130" spans="2:13" x14ac:dyDescent="0.2">
+        <v>379</v>
+      </c>
+      <c r="N129" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
         <v>151</v>
       </c>
@@ -6653,6 +6733,9 @@
       <c r="F130">
         <v>29</v>
       </c>
+      <c r="G130" t="b">
+        <v>1</v>
+      </c>
       <c r="H130" t="b">
         <v>1</v>
       </c>
@@ -6663,10 +6746,13 @@
         <v>0</v>
       </c>
       <c r="M130" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="131" spans="2:13" x14ac:dyDescent="0.2">
+        <v>395</v>
+      </c>
+      <c r="N130" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
         <v>152</v>
       </c>
@@ -6679,6 +6765,9 @@
       <c r="F131">
         <v>29</v>
       </c>
+      <c r="G131" t="b">
+        <v>1</v>
+      </c>
       <c r="H131" t="b">
         <v>1</v>
       </c>
@@ -6689,10 +6778,13 @@
         <v>0</v>
       </c>
       <c r="M131" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="132" spans="2:13" x14ac:dyDescent="0.2">
+        <v>363</v>
+      </c>
+      <c r="N131" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
         <v>153</v>
       </c>
@@ -6705,6 +6797,9 @@
       <c r="F132">
         <v>29</v>
       </c>
+      <c r="G132" t="b">
+        <v>1</v>
+      </c>
       <c r="H132" t="b">
         <v>1</v>
       </c>
@@ -6715,10 +6810,13 @@
         <v>0</v>
       </c>
       <c r="M132" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="133" spans="2:13" x14ac:dyDescent="0.2">
+        <v>369</v>
+      </c>
+      <c r="N132" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
         <v>154</v>
       </c>
@@ -6731,6 +6829,9 @@
       <c r="F133">
         <v>29</v>
       </c>
+      <c r="G133" t="b">
+        <v>1</v>
+      </c>
       <c r="H133" t="b">
         <v>1</v>
       </c>
@@ -6741,10 +6842,13 @@
         <v>0</v>
       </c>
       <c r="M133" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="134" spans="2:13" x14ac:dyDescent="0.2">
+        <v>368</v>
+      </c>
+      <c r="N133" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
         <v>155</v>
       </c>
@@ -6757,6 +6861,9 @@
       <c r="F134">
         <v>29</v>
       </c>
+      <c r="G134" t="b">
+        <v>1</v>
+      </c>
       <c r="H134" t="b">
         <v>1</v>
       </c>
@@ -6767,10 +6874,13 @@
         <v>0</v>
       </c>
       <c r="M134" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="135" spans="2:13" x14ac:dyDescent="0.2">
+        <v>365</v>
+      </c>
+      <c r="N134" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B135" t="s">
         <v>156</v>
       </c>
@@ -6783,6 +6893,9 @@
       <c r="F135">
         <v>29</v>
       </c>
+      <c r="G135" t="b">
+        <v>1</v>
+      </c>
       <c r="H135" t="b">
         <v>1</v>
       </c>
@@ -6793,10 +6906,13 @@
         <v>0</v>
       </c>
       <c r="M135" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="136" spans="2:13" x14ac:dyDescent="0.2">
+        <v>366</v>
+      </c>
+      <c r="N135" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
         <v>157</v>
       </c>
@@ -6809,6 +6925,9 @@
       <c r="F136">
         <v>29</v>
       </c>
+      <c r="G136" t="b">
+        <v>1</v>
+      </c>
       <c r="H136" t="b">
         <v>1</v>
       </c>
@@ -6819,10 +6938,13 @@
         <v>0</v>
       </c>
       <c r="M136" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="137" spans="2:13" x14ac:dyDescent="0.2">
+        <v>370</v>
+      </c>
+      <c r="N136" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B137" t="s">
         <v>158</v>
       </c>
@@ -6835,6 +6957,9 @@
       <c r="F137">
         <v>29</v>
       </c>
+      <c r="G137" t="b">
+        <v>1</v>
+      </c>
       <c r="H137" t="b">
         <v>1</v>
       </c>
@@ -6845,10 +6970,13 @@
         <v>0</v>
       </c>
       <c r="M137" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="138" spans="2:13" x14ac:dyDescent="0.2">
+        <v>371</v>
+      </c>
+      <c r="N137" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B138" t="s">
         <v>159</v>
       </c>
@@ -6861,6 +6989,9 @@
       <c r="F138">
         <v>30</v>
       </c>
+      <c r="G138" t="b">
+        <v>1</v>
+      </c>
       <c r="H138" t="b">
         <v>1</v>
       </c>
@@ -6871,10 +7002,13 @@
         <v>0</v>
       </c>
       <c r="M138" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="139" spans="2:13" x14ac:dyDescent="0.2">
+        <v>364</v>
+      </c>
+      <c r="N138" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B139" t="s">
         <v>160</v>
       </c>
@@ -6887,6 +7021,9 @@
       <c r="F139">
         <v>30</v>
       </c>
+      <c r="G139" t="b">
+        <v>1</v>
+      </c>
       <c r="H139" t="b">
         <v>1</v>
       </c>
@@ -6897,10 +7034,13 @@
         <v>0</v>
       </c>
       <c r="M139" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="140" spans="2:13" x14ac:dyDescent="0.2">
+        <v>364</v>
+      </c>
+      <c r="N139" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B140" t="s">
         <v>161</v>
       </c>
@@ -6913,6 +7053,9 @@
       <c r="F140">
         <v>30</v>
       </c>
+      <c r="G140" t="b">
+        <v>1</v>
+      </c>
       <c r="H140" t="b">
         <v>1</v>
       </c>
@@ -6923,10 +7066,13 @@
         <v>0</v>
       </c>
       <c r="M140" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="141" spans="2:13" x14ac:dyDescent="0.2">
+        <v>367</v>
+      </c>
+      <c r="N140" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B141" t="s">
         <v>162</v>
       </c>
@@ -6939,6 +7085,9 @@
       <c r="F141">
         <v>30</v>
       </c>
+      <c r="G141" t="b">
+        <v>1</v>
+      </c>
       <c r="H141" t="b">
         <v>1</v>
       </c>
@@ -6949,10 +7098,13 @@
         <v>0</v>
       </c>
       <c r="M141" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="142" spans="2:13" x14ac:dyDescent="0.2">
+        <v>367</v>
+      </c>
+      <c r="N141" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B142" t="s">
         <v>165</v>
       </c>
@@ -6965,6 +7117,9 @@
       <c r="F142">
         <v>30</v>
       </c>
+      <c r="G142" t="b">
+        <v>1</v>
+      </c>
       <c r="H142" t="b">
         <v>1</v>
       </c>
@@ -6975,10 +7130,13 @@
         <v>0</v>
       </c>
       <c r="M142" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="143" spans="2:13" x14ac:dyDescent="0.2">
+        <v>397</v>
+      </c>
+      <c r="N142" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B143" t="s">
         <v>166</v>
       </c>
@@ -6991,6 +7149,9 @@
       <c r="F143">
         <v>30</v>
       </c>
+      <c r="G143" t="b">
+        <v>1</v>
+      </c>
       <c r="H143" t="b">
         <v>1</v>
       </c>
@@ -7001,10 +7162,13 @@
         <v>0</v>
       </c>
       <c r="M143" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="144" spans="2:13" x14ac:dyDescent="0.2">
+        <v>397</v>
+      </c>
+      <c r="N143" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B144" t="s">
         <v>163</v>
       </c>
@@ -7017,6 +7181,9 @@
       <c r="F144">
         <v>30</v>
       </c>
+      <c r="G144" t="b">
+        <v>1</v>
+      </c>
       <c r="H144" t="b">
         <v>1</v>
       </c>
@@ -7027,10 +7194,13 @@
         <v>0</v>
       </c>
       <c r="M144" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="145" spans="2:13" x14ac:dyDescent="0.2">
+        <v>396</v>
+      </c>
+      <c r="N144" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B145" t="s">
         <v>164</v>
       </c>
@@ -7043,6 +7213,9 @@
       <c r="F145">
         <v>30</v>
       </c>
+      <c r="G145" t="b">
+        <v>1</v>
+      </c>
       <c r="H145" t="b">
         <v>1</v>
       </c>
@@ -7053,7 +7226,10 @@
         <v>0</v>
       </c>
       <c r="M145" t="s">
-        <v>397</v>
+        <v>396</v>
+      </c>
+      <c r="N145" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -7213,7 +7389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D8AFCC-95AF-4A6B-815E-C005352AB991}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E40" sqref="E40:E41"/>
     </sheetView>
   </sheetViews>
@@ -7302,13 +7478,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -7316,13 +7492,13 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -7330,13 +7506,13 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
+        <v>268</v>
+      </c>
+      <c r="E6" t="s">
+        <v>406</v>
+      </c>
+      <c r="G6" t="s">
         <v>269</v>
-      </c>
-      <c r="E6" t="s">
-        <v>407</v>
-      </c>
-      <c r="G6" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -7344,13 +7520,13 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E7" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -7358,13 +7534,13 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E8" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -7372,13 +7548,13 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
+        <v>268</v>
+      </c>
+      <c r="E9" t="s">
+        <v>409</v>
+      </c>
+      <c r="G9" t="s">
         <v>269</v>
-      </c>
-      <c r="E9" t="s">
-        <v>410</v>
-      </c>
-      <c r="G9" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -7386,13 +7562,13 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E10" t="s">
         <v>206</v>
       </c>
       <c r="G10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -7400,13 +7576,13 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E11" t="s">
         <v>207</v>
       </c>
       <c r="G11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -7414,13 +7590,13 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -7428,13 +7604,13 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -7442,13 +7618,13 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F14" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -7456,13 +7632,13 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F15" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -7470,13 +7646,13 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G16" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
@@ -7484,13 +7660,13 @@
         <v>14</v>
       </c>
       <c r="C17" t="s">
+        <v>295</v>
+      </c>
+      <c r="F17" t="s">
         <v>296</v>
       </c>
-      <c r="F17" t="s">
-        <v>297</v>
-      </c>
       <c r="G17" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
@@ -7498,13 +7674,13 @@
         <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G18" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
@@ -7512,13 +7688,13 @@
         <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F19" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G19" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
@@ -7526,13 +7702,13 @@
         <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F20" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G20" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
@@ -7540,13 +7716,13 @@
         <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G21" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
@@ -7554,13 +7730,13 @@
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F22" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
@@ -7568,13 +7744,13 @@
         <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F23" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G23" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
@@ -7582,13 +7758,13 @@
         <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F24" t="s">
         <v>218</v>
       </c>
       <c r="G24" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
@@ -7596,13 +7772,13 @@
         <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F25" t="s">
         <v>219</v>
       </c>
       <c r="G25" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
@@ -7610,13 +7786,13 @@
         <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F26" t="s">
         <v>218</v>
       </c>
       <c r="G26" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
@@ -7624,13 +7800,13 @@
         <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F27" t="s">
         <v>220</v>
       </c>
       <c r="G27" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
@@ -7638,13 +7814,13 @@
         <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F28" t="s">
         <v>220</v>
       </c>
       <c r="G28" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
@@ -7652,13 +7828,13 @@
         <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F29" t="s">
         <v>219</v>
       </c>
       <c r="G29" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
@@ -7666,13 +7842,13 @@
         <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F30" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G30" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.2">
@@ -7680,13 +7856,13 @@
         <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F31" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G31" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
@@ -7694,10 +7870,10 @@
         <v>29</v>
       </c>
       <c r="C32" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G32" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.2">
@@ -7705,13 +7881,13 @@
         <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F33" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G33" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.2">
@@ -7719,13 +7895,13 @@
         <v>31</v>
       </c>
       <c r="C34" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F34" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G34" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.2">
@@ -7733,10 +7909,10 @@
         <v>32</v>
       </c>
       <c r="C35" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G35" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
@@ -7744,13 +7920,13 @@
         <v>33</v>
       </c>
       <c r="C36" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F36" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G36" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
@@ -7758,13 +7934,13 @@
         <v>34</v>
       </c>
       <c r="C37" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F37" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G37" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
@@ -7772,10 +7948,10 @@
         <v>35</v>
       </c>
       <c r="C38" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G38" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.2">
@@ -7783,13 +7959,13 @@
         <v>71</v>
       </c>
       <c r="C39" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F39" t="s">
         <v>46</v>
       </c>
       <c r="G39" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.2">
@@ -7797,13 +7973,13 @@
         <v>72</v>
       </c>
       <c r="C40" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E40" t="s">
         <v>208</v>
       </c>
       <c r="G40" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.2">
@@ -7811,13 +7987,13 @@
         <v>73</v>
       </c>
       <c r="C41" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E41" t="s">
         <v>209</v>
       </c>
       <c r="G41" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.2">
@@ -7825,10 +8001,10 @@
         <v>74</v>
       </c>
       <c r="C42" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G42" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>